<commit_message>
Updating excel table for ISME
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/ISME_tables.xlsx
+++ b/Manuscript/Tables/ISME_tables.xlsx
@@ -98,25 +98,25 @@
     <t>1</t>
   </si>
   <si>
-    <t>4</t>
+    <t>5</t>
   </si>
   <si>
     <t>17459</t>
   </si>
   <si>
-    <t>1561</t>
+    <t>1552</t>
   </si>
   <si>
     <t>46</t>
   </si>
   <si>
-    <t>342</t>
-  </si>
-  <si>
-    <t>755</t>
-  </si>
-  <si>
-    <t>17</t>
+    <t>340</t>
+  </si>
+  <si>
+    <t>761</t>
+  </si>
+  <si>
+    <t>18</t>
   </si>
 </sst>
 </file>

</xml_diff>